<commit_message>
Final bugfix and polish
</commit_message>
<xml_diff>
--- a/VaultViewer/VaultViewer/DataAccessLayer/Data/HRData.xlsx
+++ b/VaultViewer/VaultViewer/DataAccessLayer/Data/HRData.xlsx
@@ -46,12 +46,6 @@
     <x:t>EmploymentDate</x:t>
   </x:si>
   <x:si>
-    <x:t>CurrentMonthlySalary</x:t>
-  </x:si>
-  <x:si>
-    <x:t>IsDeleted</x:t>
-  </x:si>
-  <x:si>
     <x:t>1</x:t>
   </x:si>
   <x:si>
@@ -82,16 +76,115 @@
     <x:t>14/04/2025 00:00:00</x:t>
   </x:si>
   <x:si>
-    <x:t>0.00</x:t>
-  </x:si>
-  <x:si>
-    <x:t>0</x:t>
-  </x:si>
-  <x:si>
     <x:t>2</x:t>
   </x:si>
   <x:si>
     <x:t>HumanResources</x:t>
+  </x:si>
+  <x:si>
+    <x:t>3</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Engineering</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Admin</x:t>
+  </x:si>
+  <x:si>
+    <x:t>5</x:t>
+  </x:si>
+  <x:si>
+    <x:t>test</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bo</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Vermote</x:t>
+  </x:si>
+  <x:si>
+    <x:t>19/05/2003 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Poperboswegel</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8000</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Brugge</x:t>
+  </x:si>
+  <x:si>
+    <x:t>12/03/2003 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>7</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Elliot</x:t>
+  </x:si>
+  <x:si>
+    <x:t>21/05/2002 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Address</x:t>
+  </x:si>
+  <x:si>
+    <x:t>City</x:t>
+  </x:si>
+  <x:si>
+    <x:t>01/05/2025 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>8</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Artyom</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Volkov</x:t>
+  </x:si>
+  <x:si>
+    <x:t>29/05/1998 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Moscow</x:t>
+  </x:si>
+  <x:si>
+    <x:t>6485</x:t>
+  </x:si>
+  <x:si>
+    <x:t>ST petersburg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>RU</x:t>
+  </x:si>
+  <x:si>
+    <x:t>07/02/2003 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>9</x:t>
+  </x:si>
+  <x:si>
+    <x:t>Bolkov</x:t>
+  </x:si>
+  <x:si>
+    <x:t>06/02/2003 00:00:00</x:t>
+  </x:si>
+  <x:si>
+    <x:t>4625</x:t>
+  </x:si>
+  <x:si>
+    <x:t>St petersburg</x:t>
+  </x:si>
+  <x:si>
+    <x:t>30/05/2025 00:00:00</x:t>
   </x:si>
 </x:sst>
 </file>
@@ -442,13 +535,13 @@
   <x:sheetPr>
     <x:outlinePr summaryBelow="1" summaryRight="1"/>
   </x:sheetPr>
-  <x:dimension ref="A1:L3"/>
+  <x:dimension ref="A1:J10"/>
   <x:sheetViews>
     <x:sheetView workbookViewId="0"/>
   </x:sheetViews>
   <x:sheetFormatPr defaultRowHeight="15"/>
   <x:sheetData>
-    <x:row r="1" spans="1:12">
+    <x:row r="1" spans="1:10">
       <x:c r="A1" s="0" t="s">
         <x:v>0</x:v>
       </x:c>
@@ -479,87 +572,293 @@
       <x:c r="J1" s="0" t="s">
         <x:v>9</x:v>
       </x:c>
-      <x:c r="K1" s="0" t="s">
+    </x:row>
+    <x:row r="2" spans="1:10">
+      <x:c r="A2" s="0" t="s">
         <x:v>10</x:v>
       </x:c>
-      <x:c r="L1" s="0" t="s">
+      <x:c r="B2" s="0" t="s">
         <x:v>11</x:v>
       </x:c>
-    </x:row>
-    <x:row r="2" spans="1:12">
-      <x:c r="A2" s="0" t="s">
+      <x:c r="C2" s="0" t="s">
         <x:v>12</x:v>
       </x:c>
-      <x:c r="B2" s="0" t="s">
+      <x:c r="D2" s="0" t="s">
         <x:v>13</x:v>
       </x:c>
-      <x:c r="C2" s="0" t="s">
+      <x:c r="E2" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D2" s="0" t="s">
+      <x:c r="F2" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="E2" s="0" t="s">
+      <x:c r="G2" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="F2" s="0" t="s">
+      <x:c r="H2" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="G2" s="0" t="s">
+      <x:c r="I2" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="H2" s="0" t="s">
+      <x:c r="J2" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="I2" s="0" t="s">
+    </x:row>
+    <x:row r="3" spans="1:10">
+      <x:c r="A3" s="0" t="s">
         <x:v>20</x:v>
       </x:c>
-      <x:c r="J2" s="0" t="s">
+      <x:c r="B3" s="0" t="s">
         <x:v>21</x:v>
       </x:c>
-      <x:c r="K2" s="0" t="s">
+      <x:c r="C3" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D3" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E3" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F3" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G3" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H3" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="I3" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J3" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="4" spans="1:10">
+      <x:c r="A4" s="0" t="s">
         <x:v>22</x:v>
       </x:c>
-      <x:c r="L2" s="0" t="s">
+      <x:c r="B4" s="0" t="s">
         <x:v>23</x:v>
       </x:c>
-    </x:row>
-    <x:row r="3" spans="1:12">
-      <x:c r="A3" s="0" t="s">
+      <x:c r="C4" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D4" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E4" s="0" t="s">
+        <x:v>14</x:v>
+      </x:c>
+      <x:c r="F4" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G4" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H4" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="I4" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J4" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="5" spans="1:10">
+      <x:c r="A5" s="0" t="s">
         <x:v>24</x:v>
       </x:c>
-      <x:c r="B3" s="0" t="s">
+      <x:c r="B5" s="0" t="s">
         <x:v>25</x:v>
       </x:c>
-      <x:c r="C3" s="0" t="s">
+      <x:c r="C5" s="0" t="s">
+        <x:v>12</x:v>
+      </x:c>
+      <x:c r="D5" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E5" s="0" t="s">
         <x:v>14</x:v>
       </x:c>
-      <x:c r="D3" s="0" t="s">
+      <x:c r="F5" s="0" t="s">
         <x:v>15</x:v>
       </x:c>
-      <x:c r="E3" s="0" t="s">
+      <x:c r="G5" s="0" t="s">
         <x:v>16</x:v>
       </x:c>
-      <x:c r="F3" s="0" t="s">
+      <x:c r="H5" s="0" t="s">
         <x:v>17</x:v>
       </x:c>
-      <x:c r="G3" s="0" t="s">
+      <x:c r="I5" s="0" t="s">
         <x:v>18</x:v>
       </x:c>
-      <x:c r="H3" s="0" t="s">
+      <x:c r="J5" s="0" t="s">
         <x:v>19</x:v>
       </x:c>
-      <x:c r="I3" s="0" t="s">
-        <x:v>20</x:v>
-      </x:c>
-      <x:c r="J3" s="0" t="s">
-        <x:v>21</x:v>
-      </x:c>
-      <x:c r="K3" s="0" t="s">
-        <x:v>22</x:v>
-      </x:c>
-      <x:c r="L3" s="0" t="s">
-        <x:v>23</x:v>
+    </x:row>
+    <x:row r="6" spans="1:10">
+      <x:c r="A6" s="0" t="s">
+        <x:v>26</x:v>
+      </x:c>
+      <x:c r="B6" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="C6" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="D6" s="0" t="s">
+        <x:v>13</x:v>
+      </x:c>
+      <x:c r="E6" s="0" t="s">
+        <x:v>27</x:v>
+      </x:c>
+      <x:c r="F6" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G6" s="0" t="s">
+        <x:v>16</x:v>
+      </x:c>
+      <x:c r="H6" s="0" t="s">
+        <x:v>17</x:v>
+      </x:c>
+      <x:c r="I6" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J6" s="0" t="s">
+        <x:v>19</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="7" spans="1:10">
+      <x:c r="A7" s="0" t="s">
+        <x:v>28</x:v>
+      </x:c>
+      <x:c r="B7" s="0" t="s">
+        <x:v>29</x:v>
+      </x:c>
+      <x:c r="C7" s="0" t="s">
+        <x:v>30</x:v>
+      </x:c>
+      <x:c r="D7" s="0" t="s">
+        <x:v>31</x:v>
+      </x:c>
+      <x:c r="E7" s="0" t="s">
+        <x:v>32</x:v>
+      </x:c>
+      <x:c r="F7" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G7" s="0" t="s">
+        <x:v>33</x:v>
+      </x:c>
+      <x:c r="H7" s="0" t="s">
+        <x:v>34</x:v>
+      </x:c>
+      <x:c r="I7" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J7" s="0" t="s">
+        <x:v>35</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="8" spans="1:10">
+      <x:c r="A8" s="0" t="s">
+        <x:v>36</x:v>
+      </x:c>
+      <x:c r="B8" s="0" t="s">
+        <x:v>37</x:v>
+      </x:c>
+      <x:c r="C8" s="0" t="s">
+        <x:v>2</x:v>
+      </x:c>
+      <x:c r="D8" s="0" t="s">
+        <x:v>38</x:v>
+      </x:c>
+      <x:c r="E8" s="0" t="s">
+        <x:v>39</x:v>
+      </x:c>
+      <x:c r="F8" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G8" s="0" t="s">
+        <x:v>6</x:v>
+      </x:c>
+      <x:c r="H8" s="0" t="s">
+        <x:v>40</x:v>
+      </x:c>
+      <x:c r="I8" s="0" t="s">
+        <x:v>18</x:v>
+      </x:c>
+      <x:c r="J8" s="0" t="s">
+        <x:v>41</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="9" spans="1:10">
+      <x:c r="A9" s="0" t="s">
+        <x:v>42</x:v>
+      </x:c>
+      <x:c r="B9" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C9" s="0" t="s">
+        <x:v>44</x:v>
+      </x:c>
+      <x:c r="D9" s="0" t="s">
+        <x:v>45</x:v>
+      </x:c>
+      <x:c r="E9" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F9" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G9" s="0" t="s">
+        <x:v>47</x:v>
+      </x:c>
+      <x:c r="H9" s="0" t="s">
+        <x:v>48</x:v>
+      </x:c>
+      <x:c r="I9" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="J9" s="0" t="s">
+        <x:v>50</x:v>
+      </x:c>
+    </x:row>
+    <x:row r="10" spans="1:10">
+      <x:c r="A10" s="0" t="s">
+        <x:v>51</x:v>
+      </x:c>
+      <x:c r="B10" s="0" t="s">
+        <x:v>43</x:v>
+      </x:c>
+      <x:c r="C10" s="0" t="s">
+        <x:v>52</x:v>
+      </x:c>
+      <x:c r="D10" s="0" t="s">
+        <x:v>53</x:v>
+      </x:c>
+      <x:c r="E10" s="0" t="s">
+        <x:v>46</x:v>
+      </x:c>
+      <x:c r="F10" s="0" t="s">
+        <x:v>15</x:v>
+      </x:c>
+      <x:c r="G10" s="0" t="s">
+        <x:v>54</x:v>
+      </x:c>
+      <x:c r="H10" s="0" t="s">
+        <x:v>55</x:v>
+      </x:c>
+      <x:c r="I10" s="0" t="s">
+        <x:v>49</x:v>
+      </x:c>
+      <x:c r="J10" s="0" t="s">
+        <x:v>56</x:v>
       </x:c>
     </x:row>
   </x:sheetData>

</xml_diff>